<commit_message>
update for new kyeword px search upax
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/TestData.xlsx
+++ b/src/main/resources/excel/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABC\IdeaProjects\uitesting\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD91FC9D-A00A-4BE1-8732-54FDFBD55259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10C067F-8BAD-4D5C-B213-A94CCF7ABF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="2280" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -25,42 +25,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>TestID</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>ExpectedUsername</t>
-  </si>
-  <si>
-    <t>SearchTerm</t>
-  </si>
-  <si>
-    <t>TC001</t>
-  </si>
-  <si>
-    <t>TC002</t>
-  </si>
-  <si>
-    <t>Zahid</t>
-  </si>
-  <si>
-    <t>TC003</t>
-  </si>
-  <si>
-    <t>SDET</t>
-  </si>
-  <si>
-    <t>zahidsdet@gmail.com</t>
-  </si>
-  <si>
-    <t>Woodbridge@2023</t>
+    <t>CBP001</t>
+  </si>
+  <si>
+    <t>CBP Login Test</t>
+  </si>
+  <si>
+    <t>CBP002</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>https://tf-sat.cbp.dhs.gov/pax/LoginPage</t>
+  </si>
+  <si>
+    <t>Login Successful</t>
+  </si>
+  <si>
+    <t>https://tf-sat.cbp.dhs.gov/uv/hotlists/ntc/traveler</t>
+  </si>
+  <si>
+    <t>Automated 1-Day Lookout Creation</t>
+  </si>
+  <si>
+    <t>Form Filled</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>EventNumber</t>
+  </si>
+  <si>
+    <t>PersonType</t>
+  </si>
+  <si>
+    <t>CBP_PXS_001</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Anika</t>
+  </si>
+  <si>
+    <t>https://sasq-sat.cbp.dhs.gov/person?query=person</t>
   </si>
 </sst>
 </file>
@@ -127,8 +160,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -410,83 +447,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G4" sqref="G4:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
+      <c r="E4" s="4"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="4">
+        <v>30057</v>
+      </c>
+      <c r="J4" s="2">
+        <v>500077368</v>
+      </c>
+      <c r="K4" s="2">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{A0397A3E-8ABF-4144-8CF2-313765DD6647}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{08515496-72FB-491C-A361-A5DD0BB83149}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D9979236-7C25-46C9-A096-8A63161D790B}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{A44E2CBE-BECB-4774-B1AA-C1E926B30C23}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{67589661-7148-4031-BE20-A730C0FABADF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update for general search grid
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/TestData.xlsx
+++ b/src/main/resources/excel/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABC\IdeaProjects\uitesting\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10C067F-8BAD-4D5C-B213-A94CCF7ABF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1662ED-FB5F-4A8A-A399-3D495A957800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2280" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>TestID</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t>https://sasq-sat.cbp.dhs.gov/person?query=person</t>
+  </si>
+  <si>
+    <t>GridTitle</t>
+  </si>
+  <si>
+    <t>SearchCriteria</t>
+  </si>
+  <si>
+    <t>SearchType</t>
+  </si>
+  <si>
+    <t>PX</t>
+  </si>
+  <si>
+    <t>first</t>
   </si>
 </sst>
 </file>
@@ -447,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:K4"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +479,7 @@
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,8 +513,17 @@
       <c r="K1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -515,7 +539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -531,7 +555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -556,6 +580,13 @@
       </c>
       <c r="K4" s="2">
         <v>408</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>